<commit_message>
monitoring senescence do7 245 and edits on contributions
</commit_message>
<xml_diff>
--- a/data/monitoringPhenology/2025Senescence.xlsx
+++ b/data/monitoringPhenology/2025Senescence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/monitoringPhenology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27623966-AB79-BE41-B23E-CB8E92587A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C8504F-0484-B946-90AD-8A4ABB0FA446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33680" yWindow="-1980" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shoot_elongation" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="465">
   <si>
     <t>tree_ID</t>
   </si>
@@ -1434,9 +1434,6 @@
   </si>
   <si>
     <t>lastleavesfell</t>
-  </si>
-  <si>
-    <t>only 4 leaves, very small</t>
   </si>
 </sst>
 </file>
@@ -2631,10 +2628,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M437"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="207" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A493" sqref="A493"/>
-      <selection pane="topRight" activeCell="N7" sqref="N7"/>
+      <selection pane="topRight" activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7566,7 +7563,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>307</v>
       </c>
@@ -7583,7 +7580,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>308</v>
       </c>
@@ -7600,7 +7597,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>309</v>
       </c>
@@ -7617,7 +7614,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>310</v>
       </c>
@@ -7634,7 +7631,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>311</v>
       </c>
@@ -7651,7 +7648,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>312</v>
       </c>
@@ -7668,7 +7665,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>313</v>
       </c>
@@ -7685,7 +7682,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>314</v>
       </c>
@@ -7702,7 +7699,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>315</v>
       </c>
@@ -7719,7 +7716,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>316</v>
       </c>
@@ -7736,7 +7733,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>317</v>
       </c>
@@ -7753,7 +7750,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>318</v>
       </c>
@@ -7770,7 +7767,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>319</v>
       </c>
@@ -7787,7 +7784,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>320</v>
       </c>
@@ -7803,11 +7800,8 @@
       <c r="E302" t="s">
         <v>286</v>
       </c>
-      <c r="F302" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>321</v>
       </c>
@@ -7824,7 +7818,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>322</v>
       </c>

</xml_diff>